<commit_message>
update test excel file fixture for content generation
</commit_message>
<xml_diff>
--- a/content/tests/test_metadata_files/test_output_category_mapping.xlsx
+++ b/content/tests/test_metadata_files/test_output_category_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivianallen/Projects/ons/ons-dp/dp-census-atlas/content/tests/test_metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2818BA64-2852-2E4A-B6A8-A1FB9381BDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48C93BE-DEA8-1A41-9952-0CD56C248F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{DD75F2EA-2766-4249-8B23-C90B17D049BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="107">
   <si>
     <t>Release</t>
   </si>
@@ -281,6 +281,84 @@
   </si>
   <si>
     <t>test_var_2_5a_4</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>test_var_2_17a</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_1</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_2</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_4</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_5</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_6</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_7</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_8</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_9</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_10</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_11</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_12</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_13</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_14</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_15</t>
+  </si>
+  <si>
+    <t>test_var_1_17a_3</t>
   </si>
 </sst>
 </file>
@@ -417,7 +495,151 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -1522,281 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8512381-0FD5-2141-8AA5-5925D8D7D7D2}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>-8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E8" s="4">
-        <v>-8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J11" s="4">
-        <v>-8</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A3:B5 E8:F8 E3:F4">
-    <cfRule type="expression" dxfId="56" priority="32" stopIfTrue="1">
-      <formula>LEN(TRIM(A3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E6">
-    <cfRule type="expression" dxfId="55" priority="29" stopIfTrue="1">
-      <formula>LEN(TRIM(E5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="54" priority="28" stopIfTrue="1">
-      <formula>LEN(TRIM(E7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="53" priority="27" stopIfTrue="1">
-      <formula>LEN(TRIM(F5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
-      <formula>LEN(TRIM(F6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="51" priority="25" stopIfTrue="1">
-      <formula>LEN(TRIM(F7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K11 J3:K3">
-    <cfRule type="expression" dxfId="50" priority="24" stopIfTrue="1">
-      <formula>LEN(TRIM(J3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="49" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(J6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="48" priority="22" stopIfTrue="1">
-      <formula>LEN(TRIM(J7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="47" priority="18" stopIfTrue="1">
-      <formula>LEN(TRIM(J8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="46" priority="17" stopIfTrue="1">
-      <formula>LEN(TRIM(J9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="expression" dxfId="45" priority="14" stopIfTrue="1">
-      <formula>LEN(TRIM(J4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="44" priority="13" stopIfTrue="1">
-      <formula>LEN(TRIM(J5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(J10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="42" priority="7" stopIfTrue="1">
-      <formula>LEN(TRIM(K4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="41" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(K5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
-      <formula>LEN(TRIM(K6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(K7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8">
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(K8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
-      <formula>LEN(TRIM(K9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(K10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="B2" location="'INDEX-filtered'!A1" display="Return to Index" xr:uid="{8CB0B5DB-DC87-B647-9EC6-CD72EDF89CAC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9AFBC0-72F1-6347-8077-E18C10556144}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1807,17 +1756,18 @@
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1832,51 +1782,87 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>-8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E5" s="4">
-        <v>2</v>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>79</v>
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E7" s="4" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1887,126 +1873,506 @@
         <v>9</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J11" s="4">
+        <v>-8</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A3:B5 E8:F8 E3:F4">
+    <cfRule type="expression" dxfId="68" priority="38" stopIfTrue="1">
+      <formula>LEN(TRIM(A3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E6">
+    <cfRule type="expression" dxfId="67" priority="35" stopIfTrue="1">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="expression" dxfId="66" priority="34" stopIfTrue="1">
+      <formula>LEN(TRIM(E7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="65" priority="33" stopIfTrue="1">
+      <formula>LEN(TRIM(F5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="64" priority="32" stopIfTrue="1">
+      <formula>LEN(TRIM(F6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="expression" dxfId="63" priority="31" stopIfTrue="1">
+      <formula>LEN(TRIM(F7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:K11 J3:K3">
+    <cfRule type="expression" dxfId="62" priority="30" stopIfTrue="1">
+      <formula>LEN(TRIM(J3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" dxfId="61" priority="29" stopIfTrue="1">
+      <formula>LEN(TRIM(J6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="expression" dxfId="60" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(J7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="expression" dxfId="59" priority="24" stopIfTrue="1">
+      <formula>LEN(TRIM(J8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="expression" dxfId="58" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(J9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="expression" dxfId="57" priority="20" stopIfTrue="1">
+      <formula>LEN(TRIM(J4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="expression" dxfId="56" priority="19" stopIfTrue="1">
+      <formula>LEN(TRIM(J5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="expression" dxfId="55" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(J10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="expression" dxfId="54" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(K4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="expression" dxfId="53" priority="12" stopIfTrue="1">
+      <formula>LEN(TRIM(K5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(K6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="expression" dxfId="51" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(K7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="expression" dxfId="50" priority="9" stopIfTrue="1">
+      <formula>LEN(TRIM(K8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="49" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(K9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="48" priority="7" stopIfTrue="1">
+      <formula>LEN(TRIM(K10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B2" location="'INDEX-filtered'!A1" display="Return to Index" xr:uid="{8CB0B5DB-DC87-B647-9EC6-CD72EDF89CAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9AFBC0-72F1-6347-8077-E18C10556144}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>-8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E8" s="4">
+        <v>-8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J13" s="4">
         <v>-8</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="M13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M18" s="4">
+        <v>-8</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E8:F8 E4:F5 A3:B4">
-    <cfRule type="expression" dxfId="35" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="26" stopIfTrue="1">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="33" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="24" stopIfTrue="1">
       <formula>LEN(TRIM(F6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="32" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(F7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:K13 J7:K7">
-    <cfRule type="expression" dxfId="31" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="21" stopIfTrue="1">
       <formula>LEN(TRIM(J7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="20" stopIfTrue="1">
       <formula>LEN(TRIM(J10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="29" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(J11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="28" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(J12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="27" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(J8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="26" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(J9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="expression" dxfId="25" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(K8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="12" stopIfTrue="1">
       <formula>LEN(TRIM(K9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(K10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="22" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(K11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="21" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(K12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:N18 M3:N4">
+    <cfRule type="expression" dxfId="26" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(M3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M6">
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
+      <formula>LEN(TRIM(M5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M17">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(M7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="expression" dxfId="23" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(N5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6">
+    <cfRule type="expression" dxfId="22" priority="2" stopIfTrue="1">
+      <formula>LEN(TRIM(N6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N17">
+    <cfRule type="expression" dxfId="21" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(N7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
refactor content scripts for new content.json format
- Refactor make_atlas_content_jsons.py to output new format

- add update_old_json_to_new.py script to update old content.json
files to match new format (needed to continue working with 2011 data)

- add validate_content_json.py script for checking content.json files
will work properly (make_atlas_content_jsons.py does this before output,
but files can/should be manually edited and so should be re-checked
subsequently)

Misc
- fix some bugs where make_atlas_content.json was aliasing
classifications that had the same suffix when parsing required
classifications (e.g. '8A' being required was picking up 8A, 18A,
98A, etc)
</commit_message>
<xml_diff>
--- a/content/tests/test_metadata_files/test_output_category_mapping.xlsx
+++ b/content/tests/test_metadata_files/test_output_category_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivianallen/Projects/ons/ons-dp/dp-census-atlas/content/tests/test_metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2818BA64-2852-2E4A-B6A8-A1FB9381BDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48C93BE-DEA8-1A41-9952-0CD56C248F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{DD75F2EA-2766-4249-8B23-C90B17D049BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="107">
   <si>
     <t>Release</t>
   </si>
@@ -281,6 +281,84 @@
   </si>
   <si>
     <t>test_var_2_5a_4</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>test_var_2_17a</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_1</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_2</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_4</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_5</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_6</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_7</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_8</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_9</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_10</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_11</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_12</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_13</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_14</t>
+  </si>
+  <si>
+    <t>test_var_2_17a_15</t>
+  </si>
+  <si>
+    <t>test_var_1_17a_3</t>
   </si>
 </sst>
 </file>
@@ -417,7 +495,151 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -1522,281 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8512381-0FD5-2141-8AA5-5925D8D7D7D2}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>-8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E8" s="4">
-        <v>-8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J11" s="4">
-        <v>-8</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A3:B5 E8:F8 E3:F4">
-    <cfRule type="expression" dxfId="56" priority="32" stopIfTrue="1">
-      <formula>LEN(TRIM(A3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E6">
-    <cfRule type="expression" dxfId="55" priority="29" stopIfTrue="1">
-      <formula>LEN(TRIM(E5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="54" priority="28" stopIfTrue="1">
-      <formula>LEN(TRIM(E7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="53" priority="27" stopIfTrue="1">
-      <formula>LEN(TRIM(F5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
-      <formula>LEN(TRIM(F6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="51" priority="25" stopIfTrue="1">
-      <formula>LEN(TRIM(F7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K11 J3:K3">
-    <cfRule type="expression" dxfId="50" priority="24" stopIfTrue="1">
-      <formula>LEN(TRIM(J3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="49" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(J6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="48" priority="22" stopIfTrue="1">
-      <formula>LEN(TRIM(J7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="47" priority="18" stopIfTrue="1">
-      <formula>LEN(TRIM(J8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="46" priority="17" stopIfTrue="1">
-      <formula>LEN(TRIM(J9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="expression" dxfId="45" priority="14" stopIfTrue="1">
-      <formula>LEN(TRIM(J4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="44" priority="13" stopIfTrue="1">
-      <formula>LEN(TRIM(J5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(J10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="42" priority="7" stopIfTrue="1">
-      <formula>LEN(TRIM(K4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="41" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(K5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
-      <formula>LEN(TRIM(K6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(K7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8">
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(K8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
-      <formula>LEN(TRIM(K9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(K10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="B2" location="'INDEX-filtered'!A1" display="Return to Index" xr:uid="{8CB0B5DB-DC87-B647-9EC6-CD72EDF89CAC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9AFBC0-72F1-6347-8077-E18C10556144}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1807,17 +1756,18 @@
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1832,51 +1782,87 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>-8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E5" s="4">
-        <v>2</v>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>79</v>
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E7" s="4" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1887,126 +1873,506 @@
         <v>9</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J11" s="4">
+        <v>-8</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A3:B5 E8:F8 E3:F4">
+    <cfRule type="expression" dxfId="68" priority="38" stopIfTrue="1">
+      <formula>LEN(TRIM(A3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E6">
+    <cfRule type="expression" dxfId="67" priority="35" stopIfTrue="1">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="expression" dxfId="66" priority="34" stopIfTrue="1">
+      <formula>LEN(TRIM(E7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="65" priority="33" stopIfTrue="1">
+      <formula>LEN(TRIM(F5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="64" priority="32" stopIfTrue="1">
+      <formula>LEN(TRIM(F6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="expression" dxfId="63" priority="31" stopIfTrue="1">
+      <formula>LEN(TRIM(F7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:K11 J3:K3">
+    <cfRule type="expression" dxfId="62" priority="30" stopIfTrue="1">
+      <formula>LEN(TRIM(J3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" dxfId="61" priority="29" stopIfTrue="1">
+      <formula>LEN(TRIM(J6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="expression" dxfId="60" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(J7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="expression" dxfId="59" priority="24" stopIfTrue="1">
+      <formula>LEN(TRIM(J8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="expression" dxfId="58" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(J9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="expression" dxfId="57" priority="20" stopIfTrue="1">
+      <formula>LEN(TRIM(J4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="expression" dxfId="56" priority="19" stopIfTrue="1">
+      <formula>LEN(TRIM(J5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="expression" dxfId="55" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(J10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="expression" dxfId="54" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(K4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="expression" dxfId="53" priority="12" stopIfTrue="1">
+      <formula>LEN(TRIM(K5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(K6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="expression" dxfId="51" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(K7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="expression" dxfId="50" priority="9" stopIfTrue="1">
+      <formula>LEN(TRIM(K8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="49" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(K9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="48" priority="7" stopIfTrue="1">
+      <formula>LEN(TRIM(K10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B2" location="'INDEX-filtered'!A1" display="Return to Index" xr:uid="{8CB0B5DB-DC87-B647-9EC6-CD72EDF89CAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9AFBC0-72F1-6347-8077-E18C10556144}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>-8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E8" s="4">
+        <v>-8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J13" s="4">
         <v>-8</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="M13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M18" s="4">
+        <v>-8</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E8:F8 E4:F5 A3:B4">
-    <cfRule type="expression" dxfId="35" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="26" stopIfTrue="1">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="33" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="24" stopIfTrue="1">
       <formula>LEN(TRIM(F6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="32" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(F7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:K13 J7:K7">
-    <cfRule type="expression" dxfId="31" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="21" stopIfTrue="1">
       <formula>LEN(TRIM(J7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="20" stopIfTrue="1">
       <formula>LEN(TRIM(J10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="29" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(J11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="28" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(J12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="27" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(J8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="26" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(J9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="expression" dxfId="25" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(K8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="12" stopIfTrue="1">
       <formula>LEN(TRIM(K9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(K10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="22" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(K11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="21" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(K12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:N18 M3:N4">
+    <cfRule type="expression" dxfId="26" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(M3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M6">
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
+      <formula>LEN(TRIM(M5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M17">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(M7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="expression" dxfId="23" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(N5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6">
+    <cfRule type="expression" dxfId="22" priority="2" stopIfTrue="1">
+      <formula>LEN(TRIM(N6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N17">
+    <cfRule type="expression" dxfId="21" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(N7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>